<commit_message>
#9 Lista de backlog atualizada
</commit_message>
<xml_diff>
--- a/Listas de Backlog para Trabalho de gestão de condomínios.xlsx
+++ b/Listas de Backlog para Trabalho de gestão de condomínios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="132">
   <si>
     <t xml:space="preserve">Item de backlog</t>
   </si>
@@ -353,6 +353,69 @@
   </si>
   <si>
     <t xml:space="preserve">Itens = (09) (01) (08) (11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acesso a o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentual de inadimplencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do condominio que se não</t>
+  </si>
+  <si>
+    <t xml:space="preserve">houver inadimplencia nos anos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anteriores deve ser 10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">senão deve ser superior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a media dos anos anteriores;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O usuario deve ter acesso a um registro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dos funcionarios e seus salarios,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">salario anual e mensal,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deve-se ter o valor do 13º salario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data de férias e suas despesas;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o usuario tambem deve ter acesso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a um fundo de reserva que deve ser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisionado para o condominio;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de todas as benfeitorias do ano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e a um fundo reservado para as mesmas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Férias e 13° salario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provisionar fundo de reserva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar todas as benfeitorias</t>
   </si>
 </sst>
 </file>
@@ -459,7 +522,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -473,6 +536,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -557,15 +624,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B84" activeCellId="0" sqref="B84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.03"/>
@@ -1172,6 +1239,141 @@
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>